<commit_message>
Complete CNA news crawler
As Title
1. Free fs path system from CNA Crawler.
2. Tag function added.
3. <a><\a> tag problem resolved.

set.xlsx is a excel file for standard tag name
</commit_message>
<xml_diff>
--- a/set.xlsx
+++ b/set.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="44">
   <si>
     <t>中央社</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>職涯</t>
+  </si>
+  <si>
+    <t>娛樂名人</t>
   </si>
 </sst>
 </file>
@@ -467,14 +470,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:Y8"/>
+  <dimension ref="A1:Y8"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>

</xml_diff>